<commit_message>
annotated and extracted L103 and several other files
</commit_message>
<xml_diff>
--- a/exports/vocab-20180914-Tisu-result-csv.xlsx
+++ b/exports/vocab-20180914-Tisu-result-csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackbowers/Box Sync/Language_Data/Mixtepec_Mixtec/exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F056D7CC-3669-F446-BF32-E8409947334C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC5831-A858-A549-874D-10B86BBEF54A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{3A004DB7-55BA-E54F-A83B-D4BC1EECCCFC}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{3A004DB7-55BA-E54F-A83B-D4BC1EECCCFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -505,6 +505,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -539,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -556,6 +564,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,13 +894,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FF7452-72C3-5D40-B570-31CCCFEF9380}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" style="5"/>
+    <col min="2" max="2" width="18.5" style="6"/>
     <col min="3" max="4" width="18.5" style="3"/>
   </cols>
   <sheetData>
@@ -997,7 +1016,7 @@
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E5" t="s">
@@ -1011,7 +1030,7 @@
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E6" t="s">
@@ -1100,7 +1119,7 @@
       <c r="A13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E13" t="s">
@@ -1179,20 +1198,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:15" s="9" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E20" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="9" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1321,7 +1341,7 @@
       <c r="A29" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="6" t="s">
         <v>102</v>
       </c>
       <c r="E29" t="s">
@@ -1346,7 +1366,7 @@
       <c r="A31" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
         <v>106</v>
       </c>
       <c r="E31" t="s">
@@ -1397,7 +1417,7 @@
       <c r="A34" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -1458,7 +1478,7 @@
       <c r="A39" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="6" t="s">
         <v>122</v>
       </c>
       <c r="E39" t="s">
@@ -1478,7 +1498,7 @@
       <c r="A40" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="6" t="s">
         <v>127</v>
       </c>
       <c r="E40" t="s">
@@ -1492,7 +1512,7 @@
       <c r="A41" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="6" t="s">
         <v>131</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1529,7 +1549,7 @@
       <c r="A43" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="6" t="s">
         <v>137</v>
       </c>
       <c r="E43" t="s">
@@ -1543,7 +1563,7 @@
       <c r="A44" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="6" t="s">
         <v>141</v>
       </c>
       <c r="E44" t="s">

</xml_diff>